<commit_message>
preparations for the first gradle run
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Smoke_GroupFeature.xlsx
+++ b/src/test/resources/data/Smoke_GroupFeature.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="AddGroup" sheetId="1" r:id="rId1"/>
@@ -373,8 +373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -397,14 +397,26 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
+      <c r="A2" s="2">
+        <v>1111111</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2018</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
+      <c r="A3" s="2">
+        <v>2222222</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2018</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -495,7 +507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>